<commit_message>
resultados de las simulaciones a h pasos adelante
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones_h_pasos/ARMA/resultados_2_escenarios_trayectorias.xlsx
+++ b/codigo_final_organizado/Simulaciones_h_pasos/ARMA/resultados_2_escenarios_trayectorias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,40 +436,60 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Paso</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Paso_H</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Config</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Proceso</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Dist</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Distribución</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Var</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Varianza</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>LSPM</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>DeepAR</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Sieve Bootstrap</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>MCPS</t>
         </is>
@@ -479,720 +499,1104 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.466261657221628</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.478661876134096</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>1.531723712863947</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1.425975406576414</v>
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.6111744155585743</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5690129033006749</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5730052269315968</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1.201523983950823</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B3" t="n">
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.510063872484103</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.407599922395201</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>1.430613825735892</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1.448835104950368</v>
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7982641221986373</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.8047924019109903</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.7807817623610386</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.614195032723387</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B4" t="n">
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.3757046319026</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.382173230254228</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>1.376863689705038</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1.426169396154013</v>
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.9393096580159003</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.9753460559848169</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9180924294796913</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1.55339842762461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B5" t="n">
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.529410946905102</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.481700982728566</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G5" t="n">
-        <v>1.442419743552197</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1.492184991615221</v>
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.025007291263254</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.030894573214066</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.994870906203779</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.42169572560623</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B6" t="n">
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.420278281851445</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.510761010100518</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>1.435970250014854</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1.493254396017263</v>
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.054460753601564</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.106563400494793</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.045970107778972</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.221353530532715</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B7" t="n">
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.409144644109964</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.442384153970085</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>1.387172239159973</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1.428243495041359</v>
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.097293137046979</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.154647576213079</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.090039591909097</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.209667467476888</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B8" t="n">
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.36195801135708</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.451558453179275</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>1.389677272855751</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1.410445033456835</v>
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.155142027906812</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.169621454458669</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1.155276149747512</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.244625098182325</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B9" t="n">
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.35589401571783</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.412949706541041</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G9" t="n">
-        <v>1.375719642655987</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>1.386030600085157</v>
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.169940661643991</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.190865662218098</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.169254292075034</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.226605208104858</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B10" t="n">
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1.301265528538343</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.358039032384561</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G10" t="n">
-        <v>1.335639884398531</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1.346469586830593</v>
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.252399958887364</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.266546071085097</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1.222134313999202</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.317835883504494</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B11" t="n">
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1.323945961547777</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.361952058559866</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G11" t="n">
-        <v>1.356933513179659</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>1.38922629714352</v>
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.235450223428725</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.249868750605592</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.223600834077432</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.406430913793212</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B12" t="n">
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1.30800028224152</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1.400071874378723</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G12" t="n">
-        <v>1.343780586913471</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>1.399947831766147</v>
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.271891588553515</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.256877278350306</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.247210047779979</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1.400005354452395</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>AR(1)</t>
-        </is>
+      <c r="B13" t="n">
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1.390379942441218</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.464908102552486</v>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>AR(1)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G13" t="n">
-        <v>1.398131540911946</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>1.449828670586564</v>
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.291545954485484</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.300755476921859</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.279704212468291</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1.433450705220343</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>1</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B14" t="n">
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.7217731520404712</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.7512244778701497</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G14" t="n">
-        <v>0.6787368306008977</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.7231191591691357</v>
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.5807452208693974</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.5862270838625597</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.5742997934231802</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.768935981943059</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B15" t="n">
+        <v>2</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.721834023486525</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.7082733278379982</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G15" t="n">
-        <v>0.7011008647288652</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.705260166021083</v>
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.6872800011247822</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.7073994127231991</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.6869048019234576</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.837710460998772</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>3</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B16" t="n">
+        <v>3</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.6939230181827919</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0.7078681704308417</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>0.6976462256655444</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>0.7134275583419879</v>
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.7751845737262328</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.7776084576783174</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.7477907242176457</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.8392929494603482</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>4</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B17" t="n">
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.7106895044420459</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.7130292939604705</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G17" t="n">
-        <v>0.718680795284068</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0.7212627013298524</v>
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.7498666204523332</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.7683464386286227</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.7692491902260258</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.785427588665414</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>5</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B18" t="n">
+        <v>5</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.7180771270849992</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0.7069662279771057</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G18" t="n">
-        <v>0.7109652840425974</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>0.7121464474799861</v>
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.815196123341815</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.7928463128615642</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.786260905047968</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.8538604943684081</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>6</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B19" t="n">
+        <v>6</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.7341833721218536</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0.7120702502456412</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G19" t="n">
-        <v>0.7152627564736087</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0.7233271348989601</v>
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.7658679165727764</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.7823641541396312</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.7691500414714666</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.8399063580974332</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>7</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B20" t="n">
+        <v>7</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.7016984716782811</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.6747276163667045</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G20" t="n">
-        <v>0.6778173315616354</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>0.7093823077674291</v>
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.8844683745335937</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.8280035854949863</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.8192360615369387</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.9048205214484814</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>8</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B21" t="n">
+        <v>8</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.7188176944537747</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.6728292808845153</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G21" t="n">
-        <v>0.6674700787867388</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>0.6971176416399421</v>
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.8046281833483129</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.8236244037769063</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.8238544791559919</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.931580750624509</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>9</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B22" t="n">
+        <v>9</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.6921518394072016</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.6537752706714822</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G22" t="n">
-        <v>0.6500790747453994</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>0.6664186973224649</v>
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.8344498381442419</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.7979095073975488</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.8099213360786117</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.8815474030533212</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>10</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B23" t="n">
+        <v>10</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.6869424576147071</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.6816953550543168</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G23" t="n">
-        <v>0.670930554758037</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>0.6930089248365482</v>
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.7769335595291581</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.7717697907758103</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.78554738639155</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.8083943848144927</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>11</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B24" t="n">
+        <v>11</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.7242384344514279</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.6952580335306642</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G24" t="n">
-        <v>0.69664851438961</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>0.7363350551797802</v>
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.7715747012345</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.7540812789764223</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.7563836297363358</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.7678117121046422</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>12</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>MA(1)</t>
-        </is>
+      <c r="B25" t="n">
+        <v>12</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>normal</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.747203649281289</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.7307182355286673</v>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
       </c>
       <c r="G25" t="n">
-        <v>0.7356625940789927</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>0.7646306849956009</v>
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.7436746546201887</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.7475210781758026</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.7562131695320573</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.7579146378071429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>